<commit_message>
Mybatis Generator로 자동생성한 VO랑 Mapper 올림.
</commit_message>
<xml_diff>
--- a/ProjectOctober/resources/표기 표준화 문서.xlsx
+++ b/ProjectOctober/resources/표기 표준화 문서.xlsx
@@ -748,7 +748,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="785">
   <si>
     <t xml:space="preserve">표기화 표준 문서 Ver 0.1 </t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -3013,9 +3013,6 @@
     <t>cpnNum</t>
   </si>
   <si>
-    <t>Specialty</t>
-  </si>
-  <si>
     <t>cardNum</t>
   </si>
   <si>
@@ -3693,10 +3690,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>count</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>status</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -4066,6 +4059,18 @@
   </si>
   <si>
     <t>VARCHAR2(10)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>subclass</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>specialty</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>svcCount</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -5300,8 +5305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F293"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A273" workbookViewId="0">
+      <selection activeCell="A297" sqref="A297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -5320,7 +5325,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="45.75" customHeight="1">
       <c r="A1" s="28" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -5330,7 +5335,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="29" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -5340,7 +5345,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="29" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B3" s="29"/>
       <c r="C3" s="29"/>
@@ -5350,24 +5355,24 @@
     </row>
     <row r="5" spans="1:6" ht="18" thickBot="1">
       <c r="A5" s="20" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B5" s="20" t="s">
+        <v>563</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>564</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="D5" s="20" t="s">
+        <v>566</v>
+      </c>
+      <c r="E5" s="20" t="s">
         <v>565</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>567</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" customHeight="1">
       <c r="A6" s="25" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B6" s="26"/>
       <c r="C6" s="26"/>
@@ -5376,7 +5381,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="11" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>145</v>
@@ -5385,7 +5390,7 @@
         <v>146</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>148</v>
@@ -5393,7 +5398,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="9" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>149</v>
@@ -5402,15 +5407,15 @@
         <v>150</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="11" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>152</v>
@@ -5419,7 +5424,7 @@
         <v>153</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>154</v>
@@ -5427,7 +5432,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="9" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>155</v>
@@ -5436,7 +5441,7 @@
         <v>156</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>154</v>
@@ -5444,7 +5449,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="11" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>157</v>
@@ -5453,7 +5458,7 @@
         <v>158</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>159</v>
@@ -5461,7 +5466,7 @@
     </row>
     <row r="12" spans="1:6" ht="17.25" thickBot="1">
       <c r="A12" s="16" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>160</v>
@@ -5470,7 +5475,7 @@
         <v>161</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="E12" s="18" t="s">
         <v>162</v>
@@ -5479,7 +5484,7 @@
     <row r="13" spans="1:6" ht="17.25" thickBot="1"/>
     <row r="14" spans="1:6">
       <c r="A14" s="25" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
@@ -5497,7 +5502,7 @@
         <v>164</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>148</v>
@@ -5505,7 +5510,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="9" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>165</v>
@@ -5514,7 +5519,7 @@
         <v>166</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>167</v>
@@ -5522,7 +5527,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="11" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>168</v>
@@ -5531,7 +5536,7 @@
         <v>169</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>170</v>
@@ -5539,7 +5544,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="9" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>171</v>
@@ -5548,7 +5553,7 @@
         <v>172</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>162</v>
@@ -5556,7 +5561,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>173</v>
@@ -5565,7 +5570,7 @@
         <v>174</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>175</v>
@@ -5573,7 +5578,7 @@
     </row>
     <row r="20" spans="1:5" ht="17.25" thickBot="1">
       <c r="A20" s="16" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B20" s="17" t="s">
         <v>176</v>
@@ -5582,7 +5587,7 @@
         <v>177</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E20" s="18" t="s">
         <v>151</v>
@@ -5591,7 +5596,7 @@
     <row r="21" spans="1:5" ht="17.25" thickBot="1"/>
     <row r="22" spans="1:5">
       <c r="A22" s="25" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B22" s="26"/>
       <c r="C22" s="26"/>
@@ -5609,10 +5614,10 @@
         <v>179</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -5626,7 +5631,7 @@
         <v>181</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E24" s="10" t="s">
         <v>148</v>
@@ -5634,7 +5639,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="11" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>492</v>
@@ -5643,7 +5648,7 @@
         <v>182</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>154</v>
@@ -5651,7 +5656,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="9" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>493</v>
@@ -5660,7 +5665,7 @@
         <v>184</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>170</v>
@@ -5668,7 +5673,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>165</v>
@@ -5677,7 +5682,7 @@
         <v>185</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>167</v>
@@ -5685,7 +5690,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="9" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>168</v>
@@ -5694,7 +5699,7 @@
         <v>186</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E28" s="10" t="s">
         <v>187</v>
@@ -5702,7 +5707,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="11" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>188</v>
@@ -5711,7 +5716,7 @@
         <v>189</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>190</v>
@@ -5719,7 +5724,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="9" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>191</v>
@@ -5728,7 +5733,7 @@
         <v>192</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="E30" s="10" t="s">
         <v>151</v>
@@ -5736,7 +5741,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="11" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>193</v>
@@ -5745,7 +5750,7 @@
         <v>194</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>151</v>
@@ -5753,7 +5758,7 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>157</v>
@@ -5762,7 +5767,7 @@
         <v>195</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E32" s="10" t="s">
         <v>159</v>
@@ -5770,7 +5775,7 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="11" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>196</v>
@@ -5779,7 +5784,7 @@
         <v>197</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E33" s="12" t="s">
         <v>151</v>
@@ -5787,7 +5792,7 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="9" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>198</v>
@@ -5796,7 +5801,7 @@
         <v>199</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>151</v>
@@ -5804,7 +5809,7 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="11" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>494</v>
@@ -5813,7 +5818,7 @@
         <v>200</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E35" s="12" t="s">
         <v>151</v>
@@ -5821,7 +5826,7 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="9" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>201</v>
@@ -5830,7 +5835,7 @@
         <v>495</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E36" s="10" t="s">
         <v>151</v>
@@ -5847,7 +5852,7 @@
         <v>204</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E37" s="12" t="s">
         <v>151</v>
@@ -5864,7 +5869,7 @@
         <v>206</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E38" s="10" t="s">
         <v>151</v>
@@ -5872,7 +5877,7 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="11" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>207</v>
@@ -5881,7 +5886,7 @@
         <v>208</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E39" s="12" t="s">
         <v>151</v>
@@ -5889,7 +5894,7 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="9" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>209</v>
@@ -5898,7 +5903,7 @@
         <v>210</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E40" s="10" t="s">
         <v>167</v>
@@ -5915,7 +5920,7 @@
         <v>212</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="E41" s="12" t="s">
         <v>213</v>
@@ -5932,7 +5937,7 @@
         <v>215</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="E42" s="10" t="s">
         <v>167</v>
@@ -5940,7 +5945,7 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="11" t="s">
-        <v>678</v>
+        <v>782</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>216</v>
@@ -5949,7 +5954,7 @@
         <v>217</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E43" s="12" t="s">
         <v>159</v>
@@ -5957,7 +5962,7 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="9" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>501</v>
@@ -5966,7 +5971,7 @@
         <v>218</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E44" s="10" t="s">
         <v>167</v>
@@ -5974,7 +5979,7 @@
     </row>
     <row r="45" spans="1:5" ht="17.25" thickBot="1">
       <c r="A45" s="13" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B45" s="14" t="s">
         <v>219</v>
@@ -5983,7 +5988,7 @@
         <v>220</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E45" s="15" t="s">
         <v>213</v>
@@ -5992,7 +5997,7 @@
     <row r="46" spans="1:5" ht="17.25" thickBot="1"/>
     <row r="47" spans="1:5">
       <c r="A47" s="25" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B47" s="26"/>
       <c r="C47" s="26"/>
@@ -6010,7 +6015,7 @@
         <v>222</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E48" s="12" t="s">
         <v>151</v>
@@ -6027,7 +6032,7 @@
         <v>224</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E49" s="18" t="s">
         <v>225</v>
@@ -6036,7 +6041,7 @@
     <row r="50" spans="1:5" ht="17.25" thickBot="1"/>
     <row r="51" spans="1:5">
       <c r="A51" s="25" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B51" s="26"/>
       <c r="C51" s="26"/>
@@ -6054,7 +6059,7 @@
         <v>227</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E52" s="12" t="s">
         <v>151</v>
@@ -6071,7 +6076,7 @@
         <v>229</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E53" s="10" t="s">
         <v>151</v>
@@ -6088,7 +6093,7 @@
         <v>231</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E54" s="12" t="s">
         <v>151</v>
@@ -6105,10 +6110,10 @@
         <v>233</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -6122,7 +6127,7 @@
         <v>235</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E56" s="12" t="s">
         <v>148</v>
@@ -6139,7 +6144,7 @@
         <v>237</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E57" s="10" t="s">
         <v>148</v>
@@ -6147,7 +6152,7 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="11" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>238</v>
@@ -6156,7 +6161,7 @@
         <v>239</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="E58" s="12" t="s">
         <v>162</v>
@@ -6164,7 +6169,7 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="9" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>240</v>
@@ -6173,7 +6178,7 @@
         <v>241</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="E59" s="10" t="s">
         <v>162</v>
@@ -6181,7 +6186,7 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="11" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>242</v>
@@ -6190,7 +6195,7 @@
         <v>243</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E60" s="12" t="s">
         <v>151</v>
@@ -6198,7 +6203,7 @@
     </row>
     <row r="61" spans="1:5" ht="17.25" thickBot="1">
       <c r="A61" s="16" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B61" s="17" t="s">
         <v>173</v>
@@ -6207,7 +6212,7 @@
         <v>244</v>
       </c>
       <c r="D61" s="17" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E61" s="18" t="s">
         <v>245</v>
@@ -6216,7 +6221,7 @@
     <row r="62" spans="1:5" ht="17.25" thickBot="1"/>
     <row r="63" spans="1:5">
       <c r="A63" s="25" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B63" s="26"/>
       <c r="C63" s="26"/>
@@ -6234,7 +6239,7 @@
         <v>247</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="E64" s="12" t="s">
         <v>151</v>
@@ -6251,7 +6256,7 @@
         <v>233</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="E65" s="10" t="s">
         <v>225</v>
@@ -6268,7 +6273,7 @@
         <v>235</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E66" s="12" t="s">
         <v>148</v>
@@ -6276,7 +6281,7 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="9" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>188</v>
@@ -6285,7 +6290,7 @@
         <v>248</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E67" s="10" t="s">
         <v>154</v>
@@ -6293,7 +6298,7 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="11" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>249</v>
@@ -6302,7 +6307,7 @@
         <v>250</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E68" s="12" t="s">
         <v>151</v>
@@ -6310,7 +6315,7 @@
     </row>
     <row r="69" spans="1:5" ht="33">
       <c r="A69" s="9" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>252</v>
@@ -6319,15 +6324,15 @@
         <v>253</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="E69" s="10" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="11" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B70" s="8" t="s">
         <v>219</v>
@@ -6336,7 +6341,7 @@
         <v>254</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E70" s="12" t="s">
         <v>213</v>
@@ -6344,7 +6349,7 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="9" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B71" s="7" t="s">
         <v>255</v>
@@ -6353,7 +6358,7 @@
         <v>256</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E71" s="10" t="s">
         <v>190</v>
@@ -6361,16 +6366,16 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="11" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>506</v>
+        <v>783</v>
       </c>
       <c r="C72" s="8" t="s">
         <v>257</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="E72" s="12" t="s">
         <v>258</v>
@@ -6378,7 +6383,7 @@
     </row>
     <row r="73" spans="1:5" ht="17.25" thickBot="1">
       <c r="A73" s="16" t="s">
-        <v>690</v>
+        <v>784</v>
       </c>
       <c r="B73" s="17" t="s">
         <v>259</v>
@@ -6387,7 +6392,7 @@
         <v>260</v>
       </c>
       <c r="D73" s="17" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E73" s="18" t="s">
         <v>151</v>
@@ -6405,7 +6410,7 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="11" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B76" s="8" t="s">
         <v>261</v>
@@ -6414,7 +6419,7 @@
         <v>262</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E76" s="12" t="s">
         <v>151</v>
@@ -6431,7 +6436,7 @@
         <v>237</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="E77" s="10" t="s">
         <v>148</v>
@@ -6439,7 +6444,7 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="11" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B78" s="8" t="s">
         <v>188</v>
@@ -6448,7 +6453,7 @@
         <v>263</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E78" s="12" t="s">
         <v>154</v>
@@ -6456,16 +6461,16 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="9" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>264</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E79" s="10" t="s">
         <v>265</v>
@@ -6473,7 +6478,7 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="11" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="B80" s="8" t="s">
         <v>266</v>
@@ -6482,7 +6487,7 @@
         <v>267</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E80" s="12" t="s">
         <v>268</v>
@@ -6490,7 +6495,7 @@
     </row>
     <row r="81" spans="1:5" ht="17.25" thickBot="1">
       <c r="A81" s="16" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="B81" s="17" t="s">
         <v>269</v>
@@ -6499,7 +6504,7 @@
         <v>270</v>
       </c>
       <c r="D81" s="17" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E81" s="18" t="s">
         <v>271</v>
@@ -6517,7 +6522,7 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="11" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B84" s="8" t="s">
         <v>272</v>
@@ -6526,7 +6531,7 @@
         <v>273</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E84" s="12" t="s">
         <v>148</v>
@@ -6534,7 +6539,7 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="9" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="B85" s="7" t="s">
         <v>274</v>
@@ -6543,7 +6548,7 @@
         <v>275</v>
       </c>
       <c r="D85" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E85" s="10" t="s">
         <v>151</v>
@@ -6551,7 +6556,7 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="11" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="B86" s="8" t="s">
         <v>276</v>
@@ -6560,7 +6565,7 @@
         <v>277</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E86" s="12" t="s">
         <v>151</v>
@@ -6568,7 +6573,7 @@
     </row>
     <row r="87" spans="1:5" ht="17.25" thickBot="1">
       <c r="A87" s="16" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="B87" s="17" t="s">
         <v>278</v>
@@ -6577,7 +6582,7 @@
         <v>279</v>
       </c>
       <c r="D87" s="17" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E87" s="18" t="s">
         <v>151</v>
@@ -6604,7 +6609,7 @@
         <v>281</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E90" s="12" t="s">
         <v>151</v>
@@ -6621,7 +6626,7 @@
         <v>233</v>
       </c>
       <c r="D91" s="7" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E91" s="10" t="s">
         <v>225</v>
@@ -6638,7 +6643,7 @@
         <v>235</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E92" s="12" t="s">
         <v>148</v>
@@ -6646,7 +6651,7 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B93" s="7" t="s">
         <v>188</v>
@@ -6655,7 +6660,7 @@
         <v>282</v>
       </c>
       <c r="D93" s="7" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E93" s="10" t="s">
         <v>154</v>
@@ -6663,7 +6668,7 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="11" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="B94" s="8" t="s">
         <v>283</v>
@@ -6672,7 +6677,7 @@
         <v>284</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E94" s="12" t="s">
         <v>225</v>
@@ -6680,7 +6685,7 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="9" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="B95" s="7" t="s">
         <v>285</v>
@@ -6689,7 +6694,7 @@
         <v>286</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E95" s="10" t="s">
         <v>151</v>
@@ -6697,7 +6702,7 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="11" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B96" s="8" t="s">
         <v>238</v>
@@ -6706,7 +6711,7 @@
         <v>287</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="E96" s="12" t="s">
         <v>162</v>
@@ -6714,7 +6719,7 @@
     </row>
     <row r="97" spans="1:5" ht="17.25" thickBot="1">
       <c r="A97" s="16" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="B97" s="17" t="s">
         <v>240</v>
@@ -6723,7 +6728,7 @@
         <v>288</v>
       </c>
       <c r="D97" s="17" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="E97" s="18" t="s">
         <v>162</v>
@@ -6750,7 +6755,7 @@
         <v>290</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="E100" s="12" t="s">
         <v>225</v>
@@ -6767,7 +6772,7 @@
         <v>181</v>
       </c>
       <c r="D101" s="7" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E101" s="10" t="s">
         <v>148</v>
@@ -6775,7 +6780,7 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="11" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B102" s="8" t="s">
         <v>291</v>
@@ -6784,7 +6789,7 @@
         <v>292</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E102" s="12" t="s">
         <v>151</v>
@@ -6792,7 +6797,7 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="9" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B103" s="7" t="s">
         <v>293</v>
@@ -6801,7 +6806,7 @@
         <v>294</v>
       </c>
       <c r="D103" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E103" s="10" t="s">
         <v>151</v>
@@ -6809,7 +6814,7 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="11" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B104" s="8" t="s">
         <v>295</v>
@@ -6818,7 +6823,7 @@
         <v>296</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E104" s="12" t="s">
         <v>151</v>
@@ -6826,7 +6831,7 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="9" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B105" s="7" t="s">
         <v>297</v>
@@ -6835,7 +6840,7 @@
         <v>298</v>
       </c>
       <c r="D105" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E105" s="10" t="s">
         <v>151</v>
@@ -6843,7 +6848,7 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="11" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B106" s="8" t="s">
         <v>299</v>
@@ -6852,7 +6857,7 @@
         <v>300</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E106" s="12" t="s">
         <v>151</v>
@@ -6860,7 +6865,7 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="9" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B107" s="7" t="s">
         <v>301</v>
@@ -6869,7 +6874,7 @@
         <v>302</v>
       </c>
       <c r="D107" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E107" s="10" t="s">
         <v>151</v>
@@ -6877,16 +6882,16 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="11" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="C108" s="8" t="s">
         <v>303</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E108" s="12" t="s">
         <v>151</v>
@@ -6894,16 +6899,16 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="9" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="C109" s="7" t="s">
         <v>304</v>
       </c>
       <c r="D109" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E109" s="10" t="s">
         <v>151</v>
@@ -6911,7 +6916,7 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="11" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B110" s="8" t="s">
         <v>305</v>
@@ -6920,7 +6925,7 @@
         <v>306</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E110" s="12" t="s">
         <v>151</v>
@@ -6928,7 +6933,7 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="9" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B111" s="7" t="s">
         <v>307</v>
@@ -6937,7 +6942,7 @@
         <v>308</v>
       </c>
       <c r="D111" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E111" s="10" t="s">
         <v>151</v>
@@ -6945,7 +6950,7 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="11" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B112" s="8" t="s">
         <v>309</v>
@@ -6954,7 +6959,7 @@
         <v>310</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E112" s="12" t="s">
         <v>151</v>
@@ -6962,7 +6967,7 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="9" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B113" s="7" t="s">
         <v>311</v>
@@ -6971,7 +6976,7 @@
         <v>312</v>
       </c>
       <c r="D113" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E113" s="10" t="s">
         <v>151</v>
@@ -6979,7 +6984,7 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="11" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B114" s="8" t="s">
         <v>313</v>
@@ -6988,7 +6993,7 @@
         <v>314</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E114" s="12" t="s">
         <v>151</v>
@@ -6996,7 +7001,7 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="9" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="B115" s="7" t="s">
         <v>315</v>
@@ -7005,7 +7010,7 @@
         <v>316</v>
       </c>
       <c r="D115" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E115" s="10" t="s">
         <v>151</v>
@@ -7013,7 +7018,7 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="11" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B116" s="8" t="s">
         <v>317</v>
@@ -7022,7 +7027,7 @@
         <v>318</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E116" s="12" t="s">
         <v>151</v>
@@ -7030,7 +7035,7 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="9" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="B117" s="7" t="s">
         <v>319</v>
@@ -7039,7 +7044,7 @@
         <v>320</v>
       </c>
       <c r="D117" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E117" s="10" t="s">
         <v>151</v>
@@ -7047,7 +7052,7 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="11" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B118" s="8" t="s">
         <v>321</v>
@@ -7056,7 +7061,7 @@
         <v>322</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E118" s="12" t="s">
         <v>151</v>
@@ -7064,7 +7069,7 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="9" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="B119" s="7" t="s">
         <v>323</v>
@@ -7073,7 +7078,7 @@
         <v>324</v>
       </c>
       <c r="D119" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E119" s="10" t="s">
         <v>151</v>
@@ -7081,7 +7086,7 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="11" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="B120" s="8" t="s">
         <v>325</v>
@@ -7090,7 +7095,7 @@
         <v>326</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E120" s="12" t="s">
         <v>151</v>
@@ -7098,7 +7103,7 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="9" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B121" s="7" t="s">
         <v>327</v>
@@ -7107,7 +7112,7 @@
         <v>328</v>
       </c>
       <c r="D121" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E121" s="10" t="s">
         <v>151</v>
@@ -7115,7 +7120,7 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="11" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B122" s="8" t="s">
         <v>329</v>
@@ -7124,7 +7129,7 @@
         <v>330</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E122" s="12" t="s">
         <v>151</v>
@@ -7132,7 +7137,7 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="9" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="B123" s="7" t="s">
         <v>331</v>
@@ -7141,7 +7146,7 @@
         <v>332</v>
       </c>
       <c r="D123" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E123" s="10" t="s">
         <v>151</v>
@@ -7149,7 +7154,7 @@
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="11" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B124" s="8" t="s">
         <v>333</v>
@@ -7158,7 +7163,7 @@
         <v>334</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E124" s="12" t="s">
         <v>151</v>
@@ -7166,7 +7171,7 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="9" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="B125" s="7" t="s">
         <v>335</v>
@@ -7175,7 +7180,7 @@
         <v>336</v>
       </c>
       <c r="D125" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E125" s="10" t="s">
         <v>151</v>
@@ -7183,7 +7188,7 @@
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="11" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="B126" s="8" t="s">
         <v>337</v>
@@ -7192,7 +7197,7 @@
         <v>338</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E126" s="12" t="s">
         <v>151</v>
@@ -7200,7 +7205,7 @@
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="9" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="B127" s="7" t="s">
         <v>339</v>
@@ -7209,7 +7214,7 @@
         <v>340</v>
       </c>
       <c r="D127" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E127" s="10" t="s">
         <v>151</v>
@@ -7217,7 +7222,7 @@
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="11" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="B128" s="8" t="s">
         <v>341</v>
@@ -7226,7 +7231,7 @@
         <v>342</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E128" s="12" t="s">
         <v>151</v>
@@ -7234,7 +7239,7 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="9" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="B129" s="7" t="s">
         <v>343</v>
@@ -7243,7 +7248,7 @@
         <v>344</v>
       </c>
       <c r="D129" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E129" s="10" t="s">
         <v>151</v>
@@ -7251,7 +7256,7 @@
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="11" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="B130" s="8" t="s">
         <v>345</v>
@@ -7260,7 +7265,7 @@
         <v>346</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E130" s="12" t="s">
         <v>151</v>
@@ -7268,7 +7273,7 @@
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="9" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="B131" s="7" t="s">
         <v>347</v>
@@ -7277,7 +7282,7 @@
         <v>348</v>
       </c>
       <c r="D131" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E131" s="10" t="s">
         <v>151</v>
@@ -7285,16 +7290,16 @@
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="11" t="s">
+        <v>520</v>
+      </c>
+      <c r="B132" s="8" t="s">
         <v>521</v>
-      </c>
-      <c r="B132" s="8" t="s">
-        <v>522</v>
       </c>
       <c r="C132" s="8" t="s">
         <v>349</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E132" s="12" t="s">
         <v>151</v>
@@ -7302,16 +7307,16 @@
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="9" t="s">
+        <v>522</v>
+      </c>
+      <c r="B133" s="7" t="s">
         <v>523</v>
-      </c>
-      <c r="B133" s="7" t="s">
-        <v>524</v>
       </c>
       <c r="C133" s="7" t="s">
         <v>350</v>
       </c>
       <c r="D133" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E133" s="10" t="s">
         <v>151</v>
@@ -7319,16 +7324,16 @@
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="B134" s="8" t="s">
         <v>525</v>
-      </c>
-      <c r="B134" s="8" t="s">
-        <v>526</v>
       </c>
       <c r="C134" s="8" t="s">
         <v>351</v>
       </c>
       <c r="D134" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E134" s="12" t="s">
         <v>151</v>
@@ -7336,16 +7341,16 @@
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="9" t="s">
+        <v>526</v>
+      </c>
+      <c r="B135" s="7" t="s">
         <v>527</v>
-      </c>
-      <c r="B135" s="7" t="s">
-        <v>528</v>
       </c>
       <c r="C135" s="7" t="s">
         <v>352</v>
       </c>
       <c r="D135" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E135" s="10" t="s">
         <v>151</v>
@@ -7353,16 +7358,16 @@
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="11" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C136" s="8" t="s">
         <v>353</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E136" s="12" t="s">
         <v>151</v>
@@ -7370,16 +7375,16 @@
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="9" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="B137" s="7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C137" s="7" t="s">
         <v>354</v>
       </c>
       <c r="D137" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E137" s="10" t="s">
         <v>151</v>
@@ -7387,7 +7392,7 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="11" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B138" s="8" t="s">
         <v>214</v>
@@ -7396,7 +7401,7 @@
         <v>355</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E138" s="12" t="s">
         <v>151</v>
@@ -7404,7 +7409,7 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="9" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B139" s="7" t="s">
         <v>356</v>
@@ -7413,7 +7418,7 @@
         <v>357</v>
       </c>
       <c r="D139" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E139" s="10" t="s">
         <v>151</v>
@@ -7421,7 +7426,7 @@
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="11" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B140" s="8" t="s">
         <v>358</v>
@@ -7430,7 +7435,7 @@
         <v>359</v>
       </c>
       <c r="D140" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E140" s="12" t="s">
         <v>151</v>
@@ -7438,7 +7443,7 @@
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="9" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B141" s="7" t="s">
         <v>360</v>
@@ -7447,7 +7452,7 @@
         <v>361</v>
       </c>
       <c r="D141" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E141" s="10" t="s">
         <v>151</v>
@@ -7455,7 +7460,7 @@
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="11" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B142" s="8" t="s">
         <v>362</v>
@@ -7464,7 +7469,7 @@
         <v>363</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E142" s="12" t="s">
         <v>151</v>
@@ -7472,7 +7477,7 @@
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="9" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B143" s="7" t="s">
         <v>364</v>
@@ -7481,7 +7486,7 @@
         <v>365</v>
       </c>
       <c r="D143" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E143" s="10" t="s">
         <v>151</v>
@@ -7489,7 +7494,7 @@
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="11" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B144" s="8" t="s">
         <v>366</v>
@@ -7498,7 +7503,7 @@
         <v>367</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E144" s="12" t="s">
         <v>151</v>
@@ -7506,7 +7511,7 @@
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="9" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B145" s="7" t="s">
         <v>368</v>
@@ -7515,7 +7520,7 @@
         <v>369</v>
       </c>
       <c r="D145" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E145" s="10" t="s">
         <v>151</v>
@@ -7523,7 +7528,7 @@
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="11" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B146" s="8" t="s">
         <v>370</v>
@@ -7532,7 +7537,7 @@
         <v>371</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E146" s="12" t="s">
         <v>151</v>
@@ -7540,7 +7545,7 @@
     </row>
     <row r="147" spans="1:5">
       <c r="A147" s="9" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B147" s="7" t="s">
         <v>372</v>
@@ -7549,7 +7554,7 @@
         <v>373</v>
       </c>
       <c r="D147" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E147" s="10" t="s">
         <v>151</v>
@@ -7557,7 +7562,7 @@
     </row>
     <row r="148" spans="1:5">
       <c r="A148" s="11" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B148" s="8" t="s">
         <v>374</v>
@@ -7566,7 +7571,7 @@
         <v>375</v>
       </c>
       <c r="D148" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E148" s="12" t="s">
         <v>151</v>
@@ -7574,7 +7579,7 @@
     </row>
     <row r="149" spans="1:5">
       <c r="A149" s="9" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B149" s="7" t="s">
         <v>376</v>
@@ -7583,7 +7588,7 @@
         <v>377</v>
       </c>
       <c r="D149" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E149" s="10" t="s">
         <v>151</v>
@@ -7591,7 +7596,7 @@
     </row>
     <row r="150" spans="1:5">
       <c r="A150" s="11" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="B150" s="8" t="s">
         <v>378</v>
@@ -7600,7 +7605,7 @@
         <v>379</v>
       </c>
       <c r="D150" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E150" s="12" t="s">
         <v>151</v>
@@ -7608,7 +7613,7 @@
     </row>
     <row r="151" spans="1:5">
       <c r="A151" s="9" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="B151" s="7" t="s">
         <v>380</v>
@@ -7617,7 +7622,7 @@
         <v>381</v>
       </c>
       <c r="D151" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E151" s="10" t="s">
         <v>151</v>
@@ -7625,7 +7630,7 @@
     </row>
     <row r="152" spans="1:5">
       <c r="A152" s="11" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="B152" s="8" t="s">
         <v>382</v>
@@ -7634,7 +7639,7 @@
         <v>383</v>
       </c>
       <c r="D152" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E152" s="12" t="s">
         <v>151</v>
@@ -7642,7 +7647,7 @@
     </row>
     <row r="153" spans="1:5">
       <c r="A153" s="9" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="B153" s="7" t="s">
         <v>384</v>
@@ -7651,7 +7656,7 @@
         <v>385</v>
       </c>
       <c r="D153" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E153" s="10" t="s">
         <v>151</v>
@@ -7659,7 +7664,7 @@
     </row>
     <row r="154" spans="1:5">
       <c r="A154" s="11" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B154" s="8" t="s">
         <v>386</v>
@@ -7668,7 +7673,7 @@
         <v>387</v>
       </c>
       <c r="D154" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E154" s="12" t="s">
         <v>151</v>
@@ -7676,7 +7681,7 @@
     </row>
     <row r="155" spans="1:5">
       <c r="A155" s="9" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="B155" s="7" t="s">
         <v>388</v>
@@ -7685,7 +7690,7 @@
         <v>389</v>
       </c>
       <c r="D155" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E155" s="10" t="s">
         <v>151</v>
@@ -7693,7 +7698,7 @@
     </row>
     <row r="156" spans="1:5">
       <c r="A156" s="11" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B156" s="8" t="s">
         <v>43</v>
@@ -7702,7 +7707,7 @@
         <v>390</v>
       </c>
       <c r="D156" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E156" s="12" t="s">
         <v>151</v>
@@ -7710,7 +7715,7 @@
     </row>
     <row r="157" spans="1:5">
       <c r="A157" s="9" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B157" s="7" t="s">
         <v>391</v>
@@ -7719,7 +7724,7 @@
         <v>392</v>
       </c>
       <c r="D157" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E157" s="10" t="s">
         <v>151</v>
@@ -7727,7 +7732,7 @@
     </row>
     <row r="158" spans="1:5">
       <c r="A158" s="11" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B158" s="8" t="s">
         <v>393</v>
@@ -7736,7 +7741,7 @@
         <v>394</v>
       </c>
       <c r="D158" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E158" s="12" t="s">
         <v>151</v>
@@ -7744,7 +7749,7 @@
     </row>
     <row r="159" spans="1:5">
       <c r="A159" s="9" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B159" s="7" t="s">
         <v>395</v>
@@ -7753,7 +7758,7 @@
         <v>396</v>
       </c>
       <c r="D159" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E159" s="10" t="s">
         <v>151</v>
@@ -7761,7 +7766,7 @@
     </row>
     <row r="160" spans="1:5">
       <c r="A160" s="11" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B160" s="8" t="s">
         <v>397</v>
@@ -7770,7 +7775,7 @@
         <v>398</v>
       </c>
       <c r="D160" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E160" s="12" t="s">
         <v>151</v>
@@ -7778,7 +7783,7 @@
     </row>
     <row r="161" spans="1:5">
       <c r="A161" s="9" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B161" s="7" t="s">
         <v>399</v>
@@ -7787,7 +7792,7 @@
         <v>400</v>
       </c>
       <c r="D161" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E161" s="10" t="s">
         <v>151</v>
@@ -7795,7 +7800,7 @@
     </row>
     <row r="162" spans="1:5" ht="17.25" thickBot="1">
       <c r="A162" s="13" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B162" s="14" t="s">
         <v>401</v>
@@ -7804,7 +7809,7 @@
         <v>402</v>
       </c>
       <c r="D162" s="14" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E162" s="15" t="s">
         <v>151</v>
@@ -7822,7 +7827,7 @@
     </row>
     <row r="165" spans="1:5">
       <c r="A165" s="11" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B165" s="8" t="s">
         <v>403</v>
@@ -7831,7 +7836,7 @@
         <v>404</v>
       </c>
       <c r="D165" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E165" s="12" t="s">
         <v>151</v>
@@ -7848,7 +7853,7 @@
         <v>237</v>
       </c>
       <c r="D166" s="7" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E166" s="10" t="s">
         <v>148</v>
@@ -7865,7 +7870,7 @@
         <v>233</v>
       </c>
       <c r="D167" s="8" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E167" s="12" t="s">
         <v>225</v>
@@ -7882,7 +7887,7 @@
         <v>235</v>
       </c>
       <c r="D168" s="7" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E168" s="10" t="s">
         <v>148</v>
@@ -7890,7 +7895,7 @@
     </row>
     <row r="169" spans="1:5">
       <c r="A169" s="11" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="B169" s="8" t="s">
         <v>405</v>
@@ -7899,7 +7904,7 @@
         <v>406</v>
       </c>
       <c r="D169" s="8" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="E169" s="12" t="s">
         <v>162</v>
@@ -7907,7 +7912,7 @@
     </row>
     <row r="170" spans="1:5">
       <c r="A170" s="9" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B170" s="7" t="s">
         <v>407</v>
@@ -7916,15 +7921,15 @@
         <v>408</v>
       </c>
       <c r="D170" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="E170" s="10" t="s">
         <v>616</v>
-      </c>
-      <c r="E170" s="10" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="171" spans="1:5">
       <c r="A171" s="11" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B171" s="8" t="s">
         <v>409</v>
@@ -7933,7 +7938,7 @@
         <v>410</v>
       </c>
       <c r="D171" s="8" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E171" s="12" t="s">
         <v>411</v>
@@ -7941,7 +7946,7 @@
     </row>
     <row r="172" spans="1:5">
       <c r="A172" s="9" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B172" s="7" t="s">
         <v>412</v>
@@ -7950,7 +7955,7 @@
         <v>413</v>
       </c>
       <c r="D172" s="7" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E172" s="10" t="s">
         <v>154</v>
@@ -7958,7 +7963,7 @@
     </row>
     <row r="173" spans="1:5">
       <c r="A173" s="11" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B173" s="8" t="s">
         <v>414</v>
@@ -7967,7 +7972,7 @@
         <v>415</v>
       </c>
       <c r="D173" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E173" s="12" t="s">
         <v>151</v>
@@ -7975,7 +7980,7 @@
     </row>
     <row r="174" spans="1:5">
       <c r="A174" s="9" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="B174" s="7" t="s">
         <v>416</v>
@@ -7984,7 +7989,7 @@
         <v>417</v>
       </c>
       <c r="D174" s="7" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="E174" s="10" t="s">
         <v>151</v>
@@ -7992,7 +7997,7 @@
     </row>
     <row r="175" spans="1:5">
       <c r="A175" s="11" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="B175" s="8" t="s">
         <v>418</v>
@@ -8001,7 +8006,7 @@
         <v>419</v>
       </c>
       <c r="D175" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E175" s="12" t="s">
         <v>151</v>
@@ -8009,7 +8014,7 @@
     </row>
     <row r="176" spans="1:5">
       <c r="A176" s="9" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="B176" s="7" t="s">
         <v>420</v>
@@ -8018,7 +8023,7 @@
         <v>421</v>
       </c>
       <c r="D176" s="7" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E176" s="10" t="s">
         <v>151</v>
@@ -8035,7 +8040,7 @@
         <v>31</v>
       </c>
       <c r="D177" s="14" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E177" s="15" t="s">
         <v>151</v>
@@ -8053,7 +8058,7 @@
     </row>
     <row r="180" spans="1:5">
       <c r="A180" s="11" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B180" s="8" t="s">
         <v>422</v>
@@ -8062,7 +8067,7 @@
         <v>423</v>
       </c>
       <c r="D180" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E180" s="12" t="s">
         <v>151</v>
@@ -8079,7 +8084,7 @@
         <v>233</v>
       </c>
       <c r="D181" s="7" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="E181" s="10" t="s">
         <v>225</v>
@@ -8096,7 +8101,7 @@
         <v>235</v>
       </c>
       <c r="D182" s="8" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E182" s="12" t="s">
         <v>148</v>
@@ -8104,7 +8109,7 @@
     </row>
     <row r="183" spans="1:5">
       <c r="A183" s="9" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="B183" s="7" t="s">
         <v>424</v>
@@ -8113,7 +8118,7 @@
         <v>425</v>
       </c>
       <c r="D183" s="7" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="E183" s="10" t="s">
         <v>258</v>
@@ -8121,7 +8126,7 @@
     </row>
     <row r="184" spans="1:5">
       <c r="A184" s="11" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B184" s="8" t="s">
         <v>219</v>
@@ -8130,7 +8135,7 @@
         <v>426</v>
       </c>
       <c r="D184" s="8" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E184" s="12" t="s">
         <v>258</v>
@@ -8138,7 +8143,7 @@
     </row>
     <row r="185" spans="1:5">
       <c r="A185" s="9" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="B185" s="7" t="s">
         <v>165</v>
@@ -8147,7 +8152,7 @@
         <v>427</v>
       </c>
       <c r="D185" s="7" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E185" s="10" t="s">
         <v>167</v>
@@ -8155,19 +8160,19 @@
     </row>
     <row r="186" spans="1:5" ht="17.25" thickBot="1">
       <c r="A186" s="13" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B186" s="14" t="s">
+        <v>619</v>
+      </c>
+      <c r="C186" s="14" t="s">
         <v>620</v>
       </c>
-      <c r="C186" s="14" t="s">
+      <c r="D186" s="14" t="s">
+        <v>767</v>
+      </c>
+      <c r="E186" s="15" t="s">
         <v>621</v>
-      </c>
-      <c r="D186" s="14" t="s">
-        <v>769</v>
-      </c>
-      <c r="E186" s="15" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="187" spans="1:5" ht="17.25" thickBot="1"/>
@@ -8182,7 +8187,7 @@
     </row>
     <row r="189" spans="1:5">
       <c r="A189" s="11" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B189" s="8" t="s">
         <v>428</v>
@@ -8191,7 +8196,7 @@
         <v>429</v>
       </c>
       <c r="D189" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E189" s="12" t="s">
         <v>151</v>
@@ -8208,7 +8213,7 @@
         <v>431</v>
       </c>
       <c r="D190" s="7" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E190" s="10" t="s">
         <v>151</v>
@@ -8216,7 +8221,7 @@
     </row>
     <row r="191" spans="1:5">
       <c r="A191" s="11" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="B191" s="8" t="s">
         <v>252</v>
@@ -8225,7 +8230,7 @@
         <v>432</v>
       </c>
       <c r="D191" s="8" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="E191" s="12" t="s">
         <v>162</v>
@@ -8233,7 +8238,7 @@
     </row>
     <row r="192" spans="1:5" ht="17.25" thickBot="1">
       <c r="A192" s="16" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="B192" s="17" t="s">
         <v>433</v>
@@ -8242,7 +8247,7 @@
         <v>434</v>
       </c>
       <c r="D192" s="17" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E192" s="18" t="s">
         <v>151</v>
@@ -8260,7 +8265,7 @@
     </row>
     <row r="195" spans="1:5">
       <c r="A195" s="11" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B195" s="8" t="s">
         <v>435</v>
@@ -8269,7 +8274,7 @@
         <v>436</v>
       </c>
       <c r="D195" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E195" s="12" t="s">
         <v>151</v>
@@ -8277,7 +8282,7 @@
     </row>
     <row r="196" spans="1:5">
       <c r="A196" s="9" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B196" s="7" t="s">
         <v>152</v>
@@ -8286,7 +8291,7 @@
         <v>153</v>
       </c>
       <c r="D196" s="7" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E196" s="10" t="s">
         <v>154</v>
@@ -8294,7 +8299,7 @@
     </row>
     <row r="197" spans="1:5">
       <c r="A197" s="11" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B197" s="8" t="s">
         <v>437</v>
@@ -8303,7 +8308,7 @@
         <v>147</v>
       </c>
       <c r="D197" s="8" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E197" s="12" t="s">
         <v>148</v>
@@ -8311,7 +8316,7 @@
     </row>
     <row r="198" spans="1:5" ht="17.25" thickBot="1">
       <c r="A198" s="16" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="B198" s="17" t="s">
         <v>157</v>
@@ -8320,7 +8325,7 @@
         <v>158</v>
       </c>
       <c r="D198" s="17" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E198" s="18" t="s">
         <v>159</v>
@@ -8338,7 +8343,7 @@
     </row>
     <row r="201" spans="1:5">
       <c r="A201" s="11" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B201" s="8" t="s">
         <v>438</v>
@@ -8347,7 +8352,7 @@
         <v>439</v>
       </c>
       <c r="D201" s="8" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E201" s="12" t="s">
         <v>151</v>
@@ -8364,7 +8369,7 @@
         <v>290</v>
       </c>
       <c r="D202" s="7" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E202" s="10" t="s">
         <v>225</v>
@@ -8381,7 +8386,7 @@
         <v>273</v>
       </c>
       <c r="D203" s="8" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E203" s="12" t="s">
         <v>148</v>
@@ -8389,19 +8394,19 @@
     </row>
     <row r="204" spans="1:5" ht="17.25" thickBot="1">
       <c r="A204" s="16" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="B204" s="17" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C204" s="17" t="s">
         <v>440</v>
       </c>
       <c r="D204" s="17" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="E204" s="18" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
     </row>
     <row r="205" spans="1:5" ht="17.25" thickBot="1"/>
@@ -8425,7 +8430,7 @@
         <v>290</v>
       </c>
       <c r="D207" s="8" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E207" s="12" t="s">
         <v>225</v>
@@ -8442,7 +8447,7 @@
         <v>181</v>
       </c>
       <c r="D208" s="7" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E208" s="10" t="s">
         <v>148</v>
@@ -8450,7 +8455,7 @@
     </row>
     <row r="209" spans="1:5">
       <c r="A209" s="11" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="B209" s="8" t="s">
         <v>441</v>
@@ -8459,7 +8464,7 @@
         <v>442</v>
       </c>
       <c r="D209" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E209" s="12" t="s">
         <v>151</v>
@@ -8467,7 +8472,7 @@
     </row>
     <row r="210" spans="1:5">
       <c r="A210" s="9" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="B210" s="7" t="s">
         <v>443</v>
@@ -8476,7 +8481,7 @@
         <v>444</v>
       </c>
       <c r="D210" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E210" s="10" t="s">
         <v>151</v>
@@ -8484,7 +8489,7 @@
     </row>
     <row r="211" spans="1:5">
       <c r="A211" s="11" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="B211" s="8" t="s">
         <v>445</v>
@@ -8493,7 +8498,7 @@
         <v>446</v>
       </c>
       <c r="D211" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E211" s="12" t="s">
         <v>151</v>
@@ -8501,7 +8506,7 @@
     </row>
     <row r="212" spans="1:5">
       <c r="A212" s="9" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="B212" s="7" t="s">
         <v>447</v>
@@ -8510,7 +8515,7 @@
         <v>448</v>
       </c>
       <c r="D212" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E212" s="10" t="s">
         <v>151</v>
@@ -8518,7 +8523,7 @@
     </row>
     <row r="213" spans="1:5">
       <c r="A213" s="11" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="B213" s="8" t="s">
         <v>449</v>
@@ -8527,7 +8532,7 @@
         <v>450</v>
       </c>
       <c r="D213" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E213" s="12" t="s">
         <v>151</v>
@@ -8535,7 +8540,7 @@
     </row>
     <row r="214" spans="1:5">
       <c r="A214" s="9" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B214" s="7" t="s">
         <v>451</v>
@@ -8544,7 +8549,7 @@
         <v>452</v>
       </c>
       <c r="D214" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E214" s="10" t="s">
         <v>151</v>
@@ -8552,7 +8557,7 @@
     </row>
     <row r="215" spans="1:5" ht="17.25" thickBot="1">
       <c r="A215" s="13" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="B215" s="14" t="s">
         <v>453</v>
@@ -8561,7 +8566,7 @@
         <v>454</v>
       </c>
       <c r="D215" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E215" s="15" t="s">
         <v>151</v>
@@ -8579,16 +8584,16 @@
     </row>
     <row r="218" spans="1:5">
       <c r="A218" s="11" t="s">
+        <v>557</v>
+      </c>
+      <c r="B218" s="8" t="s">
         <v>558</v>
-      </c>
-      <c r="B218" s="8" t="s">
-        <v>559</v>
       </c>
       <c r="C218" s="8" t="s">
         <v>455</v>
       </c>
       <c r="D218" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E218" s="12" t="s">
         <v>151</v>
@@ -8605,7 +8610,7 @@
         <v>233</v>
       </c>
       <c r="D219" s="7" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="E219" s="10" t="s">
         <v>225</v>
@@ -8622,7 +8627,7 @@
         <v>235</v>
       </c>
       <c r="D220" s="8" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="E220" s="12" t="s">
         <v>148</v>
@@ -8630,7 +8635,7 @@
     </row>
     <row r="221" spans="1:5" ht="17.25" thickBot="1">
       <c r="A221" s="16" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B221" s="17" t="s">
         <v>456</v>
@@ -8639,7 +8644,7 @@
         <v>457</v>
       </c>
       <c r="D221" s="17" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="E221" s="18" t="s">
         <v>162</v>
@@ -8657,7 +8662,7 @@
     </row>
     <row r="224" spans="1:5">
       <c r="A224" s="11" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B224" s="8" t="s">
         <v>458</v>
@@ -8666,7 +8671,7 @@
         <v>459</v>
       </c>
       <c r="D224" s="8" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="E224" s="12" t="s">
         <v>151</v>
@@ -8674,7 +8679,7 @@
     </row>
     <row r="225" spans="1:5">
       <c r="A225" s="9" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B225" s="7" t="s">
         <v>460</v>
@@ -8683,7 +8688,7 @@
         <v>461</v>
       </c>
       <c r="D225" s="7" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E225" s="10" t="s">
         <v>151</v>
@@ -8700,7 +8705,7 @@
         <v>233</v>
       </c>
       <c r="D226" s="8" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="E226" s="12" t="s">
         <v>225</v>
@@ -8717,7 +8722,7 @@
         <v>235</v>
       </c>
       <c r="D227" s="7" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E227" s="10" t="s">
         <v>148</v>
@@ -8725,7 +8730,7 @@
     </row>
     <row r="228" spans="1:5">
       <c r="A228" s="11" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B228" s="8" t="s">
         <v>252</v>
@@ -8734,7 +8739,7 @@
         <v>462</v>
       </c>
       <c r="D228" s="8" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="E228" s="12" t="s">
         <v>162</v>
@@ -8742,7 +8747,7 @@
     </row>
     <row r="229" spans="1:5" ht="17.25" thickBot="1">
       <c r="A229" s="16" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="B229" s="17" t="s">
         <v>433</v>
@@ -8751,7 +8756,7 @@
         <v>251</v>
       </c>
       <c r="D229" s="17" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E229" s="18" t="s">
         <v>151</v>
@@ -8778,7 +8783,7 @@
         <v>179</v>
       </c>
       <c r="D232" s="8" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="E232" s="12" t="s">
         <v>225</v>
@@ -8795,7 +8800,7 @@
         <v>146</v>
       </c>
       <c r="D233" s="7" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E233" s="10" t="s">
         <v>148</v>
@@ -8803,16 +8808,16 @@
     </row>
     <row r="234" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A234" s="11" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B234" s="8" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C234" s="8" t="s">
         <v>182</v>
       </c>
       <c r="D234" s="8" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E234" s="12" t="s">
         <v>154</v>
@@ -8820,7 +8825,7 @@
     </row>
     <row r="235" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A235" s="9" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B235" s="7" t="s">
         <v>183</v>
@@ -8829,7 +8834,7 @@
         <v>184</v>
       </c>
       <c r="D235" s="7" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E235" s="10" t="s">
         <v>170</v>
@@ -8837,7 +8842,7 @@
     </row>
     <row r="236" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A236" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B236" s="8" t="s">
         <v>165</v>
@@ -8846,7 +8851,7 @@
         <v>185</v>
       </c>
       <c r="D236" s="8" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E236" s="12" t="s">
         <v>167</v>
@@ -8854,7 +8859,7 @@
     </row>
     <row r="237" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A237" s="9" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="B237" s="7" t="s">
         <v>188</v>
@@ -8863,7 +8868,7 @@
         <v>189</v>
       </c>
       <c r="D237" s="7" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E237" s="10" t="s">
         <v>190</v>
@@ -8871,7 +8876,7 @@
     </row>
     <row r="238" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A238" s="11" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B238" s="8" t="s">
         <v>168</v>
@@ -8880,7 +8885,7 @@
         <v>186</v>
       </c>
       <c r="D238" s="8" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E238" s="12" t="s">
         <v>187</v>
@@ -8888,7 +8893,7 @@
     </row>
     <row r="239" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A239" s="9" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B239" s="7" t="s">
         <v>191</v>
@@ -8897,7 +8902,7 @@
         <v>192</v>
       </c>
       <c r="D239" s="7" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="E239" s="10" t="s">
         <v>162</v>
@@ -8905,7 +8910,7 @@
     </row>
     <row r="240" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A240" s="11" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B240" s="8" t="s">
         <v>193</v>
@@ -8914,7 +8919,7 @@
         <v>194</v>
       </c>
       <c r="D240" s="8" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="E240" s="12" t="s">
         <v>162</v>
@@ -8922,7 +8927,7 @@
     </row>
     <row r="241" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A241" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B241" s="7" t="s">
         <v>157</v>
@@ -8931,7 +8936,7 @@
         <v>195</v>
       </c>
       <c r="D241" s="7" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E241" s="10" t="s">
         <v>159</v>
@@ -8939,7 +8944,7 @@
     </row>
     <row r="242" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A242" s="11" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B242" s="8" t="s">
         <v>196</v>
@@ -8948,7 +8953,7 @@
         <v>197</v>
       </c>
       <c r="D242" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E242" s="12" t="s">
         <v>151</v>
@@ -8956,7 +8961,7 @@
     </row>
     <row r="243" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A243" s="9" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B243" s="7" t="s">
         <v>198</v>
@@ -8965,7 +8970,7 @@
         <v>199</v>
       </c>
       <c r="D243" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E243" s="10" t="s">
         <v>151</v>
@@ -8973,16 +8978,16 @@
     </row>
     <row r="244" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A244" s="11" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B244" s="8" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C244" s="8" t="s">
         <v>464</v>
       </c>
       <c r="D244" s="8" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E244" s="12" t="s">
         <v>151</v>
@@ -8990,7 +8995,7 @@
     </row>
     <row r="245" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A245" s="9" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B245" s="7" t="s">
         <v>201</v>
@@ -8999,7 +9004,7 @@
         <v>202</v>
       </c>
       <c r="D245" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E245" s="10" t="s">
         <v>151</v>
@@ -9016,7 +9021,7 @@
         <v>204</v>
       </c>
       <c r="D246" s="8" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E246" s="12" t="s">
         <v>151</v>
@@ -9033,7 +9038,7 @@
         <v>206</v>
       </c>
       <c r="D247" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E247" s="10" t="s">
         <v>151</v>
@@ -9041,7 +9046,7 @@
     </row>
     <row r="248" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A248" s="11" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B248" s="8" t="s">
         <v>207</v>
@@ -9050,7 +9055,7 @@
         <v>208</v>
       </c>
       <c r="D248" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E248" s="12" t="s">
         <v>151</v>
@@ -9058,7 +9063,7 @@
     </row>
     <row r="249" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A249" s="9" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B249" s="7" t="s">
         <v>209</v>
@@ -9067,7 +9072,7 @@
         <v>210</v>
       </c>
       <c r="D249" s="7" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E249" s="10" t="s">
         <v>167</v>
@@ -9084,7 +9089,7 @@
         <v>212</v>
       </c>
       <c r="D250" s="8" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="E250" s="12" t="s">
         <v>213</v>
@@ -9101,7 +9106,7 @@
         <v>215</v>
       </c>
       <c r="D251" s="7" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="E251" s="10" t="s">
         <v>167</v>
@@ -9109,7 +9114,7 @@
     </row>
     <row r="252" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A252" s="11" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B252" s="8" t="s">
         <v>216</v>
@@ -9118,7 +9123,7 @@
         <v>217</v>
       </c>
       <c r="D252" s="8" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E252" s="12" t="s">
         <v>159</v>
@@ -9126,16 +9131,16 @@
     </row>
     <row r="253" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A253" s="9" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B253" s="7" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C253" s="7" t="s">
         <v>218</v>
       </c>
       <c r="D253" s="7" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="E253" s="10" t="s">
         <v>167</v>
@@ -9143,7 +9148,7 @@
     </row>
     <row r="254" spans="1:5" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A254" s="13" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B254" s="14" t="s">
         <v>219</v>
@@ -9152,7 +9157,7 @@
         <v>220</v>
       </c>
       <c r="D254" s="14" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E254" s="15" t="s">
         <v>213</v>
@@ -9179,7 +9184,7 @@
         <v>290</v>
       </c>
       <c r="D257" s="8" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="E257" s="12" t="s">
         <v>225</v>
@@ -9196,7 +9201,7 @@
         <v>273</v>
       </c>
       <c r="D258" s="7" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E258" s="10" t="s">
         <v>148</v>
@@ -9204,7 +9209,7 @@
     </row>
     <row r="259" spans="1:5">
       <c r="A259" s="11" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="B259" s="8" t="s">
         <v>441</v>
@@ -9213,7 +9218,7 @@
         <v>442</v>
       </c>
       <c r="D259" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E259" s="12" t="s">
         <v>151</v>
@@ -9221,7 +9226,7 @@
     </row>
     <row r="260" spans="1:5">
       <c r="A260" s="9" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="B260" s="7" t="s">
         <v>443</v>
@@ -9230,7 +9235,7 @@
         <v>444</v>
       </c>
       <c r="D260" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E260" s="10" t="s">
         <v>151</v>
@@ -9238,7 +9243,7 @@
     </row>
     <row r="261" spans="1:5">
       <c r="A261" s="11" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="B261" s="8" t="s">
         <v>445</v>
@@ -9247,7 +9252,7 @@
         <v>446</v>
       </c>
       <c r="D261" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E261" s="12" t="s">
         <v>151</v>
@@ -9255,7 +9260,7 @@
     </row>
     <row r="262" spans="1:5">
       <c r="A262" s="9" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="B262" s="7" t="s">
         <v>447</v>
@@ -9264,7 +9269,7 @@
         <v>448</v>
       </c>
       <c r="D262" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E262" s="10" t="s">
         <v>151</v>
@@ -9272,7 +9277,7 @@
     </row>
     <row r="263" spans="1:5">
       <c r="A263" s="11" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="B263" s="8" t="s">
         <v>449</v>
@@ -9281,7 +9286,7 @@
         <v>450</v>
       </c>
       <c r="D263" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E263" s="12" t="s">
         <v>151</v>
@@ -9289,7 +9294,7 @@
     </row>
     <row r="264" spans="1:5">
       <c r="A264" s="9" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="B264" s="7" t="s">
         <v>451</v>
@@ -9298,7 +9303,7 @@
         <v>452</v>
       </c>
       <c r="D264" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E264" s="10" t="s">
         <v>151</v>
@@ -9306,7 +9311,7 @@
     </row>
     <row r="265" spans="1:5" ht="17.25" thickBot="1">
       <c r="A265" s="13" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="B265" s="14" t="s">
         <v>453</v>
@@ -9315,7 +9320,7 @@
         <v>454</v>
       </c>
       <c r="D265" s="14" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E265" s="15" t="s">
         <v>151</v>
@@ -9333,7 +9338,7 @@
     </row>
     <row r="268" spans="1:5">
       <c r="A268" s="11" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="B268" s="8" t="s">
         <v>465</v>
@@ -9342,7 +9347,7 @@
         <v>455</v>
       </c>
       <c r="D268" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E268" s="12" t="s">
         <v>151</v>
@@ -9359,7 +9364,7 @@
         <v>233</v>
       </c>
       <c r="D269" s="7" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E269" s="10" t="s">
         <v>225</v>
@@ -9376,7 +9381,7 @@
         <v>466</v>
       </c>
       <c r="D270" s="8" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="E270" s="12" t="s">
         <v>148</v>
@@ -9384,7 +9389,7 @@
     </row>
     <row r="271" spans="1:5" ht="17.25" thickBot="1">
       <c r="A271" s="16" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="B271" s="17" t="s">
         <v>467</v>
@@ -9393,7 +9398,7 @@
         <v>457</v>
       </c>
       <c r="D271" s="17" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="E271" s="18" t="s">
         <v>162</v>
@@ -9411,7 +9416,7 @@
     </row>
     <row r="274" spans="1:5">
       <c r="A274" s="11" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="B274" s="8" t="s">
         <v>468</v>
@@ -9420,7 +9425,7 @@
         <v>469</v>
       </c>
       <c r="D274" s="8" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E274" s="12" t="s">
         <v>151</v>
@@ -9437,7 +9442,7 @@
         <v>431</v>
       </c>
       <c r="D275" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E275" s="10" t="s">
         <v>151</v>
@@ -9445,7 +9450,7 @@
     </row>
     <row r="276" spans="1:5">
       <c r="A276" s="11" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B276" s="8" t="s">
         <v>470</v>
@@ -9454,7 +9459,7 @@
         <v>471</v>
       </c>
       <c r="D276" s="8" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E276" s="12" t="s">
         <v>151</v>
@@ -9462,7 +9467,7 @@
     </row>
     <row r="277" spans="1:5" ht="17.25" thickBot="1">
       <c r="A277" s="16" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B277" s="17" t="s">
         <v>155</v>
@@ -9471,7 +9476,7 @@
         <v>472</v>
       </c>
       <c r="D277" s="17" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E277" s="18" t="s">
         <v>170</v>
@@ -9498,7 +9503,7 @@
         <v>474</v>
       </c>
       <c r="D280" s="8" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E280" s="12" t="s">
         <v>187</v>
@@ -9515,7 +9520,7 @@
         <v>476</v>
       </c>
       <c r="D281" s="7" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E281" s="10" t="s">
         <v>167</v>
@@ -9532,7 +9537,7 @@
         <v>478</v>
       </c>
       <c r="D282" s="8" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E282" s="12" t="s">
         <v>167</v>
@@ -9540,33 +9545,33 @@
     </row>
     <row r="283" spans="1:5">
       <c r="A283" s="11" t="s">
+        <v>640</v>
+      </c>
+      <c r="B283" s="8" t="s">
         <v>641</v>
       </c>
-      <c r="B283" s="8" t="s">
+      <c r="C283" s="8" t="s">
         <v>642</v>
       </c>
-      <c r="C283" s="8" t="s">
+      <c r="D283" s="8" t="s">
         <v>643</v>
       </c>
-      <c r="D283" s="8" t="s">
+      <c r="E283" s="12" t="s">
         <v>644</v>
-      </c>
-      <c r="E283" s="12" t="s">
-        <v>645</v>
       </c>
     </row>
     <row r="284" spans="1:5" ht="17.25" thickBot="1">
       <c r="A284" s="16" t="s">
+        <v>645</v>
+      </c>
+      <c r="B284" s="17" t="s">
         <v>646</v>
       </c>
-      <c r="B284" s="17" t="s">
+      <c r="C284" s="17" t="s">
         <v>647</v>
       </c>
-      <c r="C284" s="17" t="s">
-        <v>648</v>
-      </c>
       <c r="D284" s="17" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E284" s="18" t="s">
         <v>167</v>
@@ -9584,16 +9589,16 @@
     </row>
     <row r="287" spans="1:5">
       <c r="A287" s="11" t="s">
+        <v>561</v>
+      </c>
+      <c r="B287" s="8" t="s">
         <v>562</v>
-      </c>
-      <c r="B287" s="8" t="s">
-        <v>563</v>
       </c>
       <c r="C287" s="8" t="s">
         <v>479</v>
       </c>
       <c r="D287" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E287" s="12" t="s">
         <v>151</v>
@@ -9610,7 +9615,7 @@
         <v>431</v>
       </c>
       <c r="D288" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E288" s="10" t="s">
         <v>151</v>
@@ -9627,7 +9632,7 @@
         <v>237</v>
       </c>
       <c r="D289" s="8" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E289" s="12" t="s">
         <v>148</v>
@@ -9644,7 +9649,7 @@
         <v>233</v>
       </c>
       <c r="D290" s="7" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="E290" s="10" t="s">
         <v>225</v>
@@ -9661,7 +9666,7 @@
         <v>235</v>
       </c>
       <c r="D291" s="8" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E291" s="12" t="s">
         <v>148</v>
@@ -9678,7 +9683,7 @@
         <v>481</v>
       </c>
       <c r="D292" s="7" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E292" s="10" t="s">
         <v>167</v>
@@ -9686,7 +9691,7 @@
     </row>
     <row r="293" spans="1:5" ht="17.25" thickBot="1">
       <c r="A293" s="13" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="B293" s="14" t="s">
         <v>482</v>
@@ -9695,7 +9700,7 @@
         <v>483</v>
       </c>
       <c r="D293" s="14" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E293" s="15" t="s">
         <v>151</v>
@@ -9703,17 +9708,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A217:E217"/>
-    <mergeCell ref="A63:E63"/>
-    <mergeCell ref="A75:E75"/>
-    <mergeCell ref="A83:E83"/>
-    <mergeCell ref="A89:E89"/>
-    <mergeCell ref="A206:E206"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="A51:E51"/>
     <mergeCell ref="A286:E286"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
@@ -9730,6 +9724,17 @@
     <mergeCell ref="A188:E188"/>
     <mergeCell ref="A194:E194"/>
     <mergeCell ref="A200:E200"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="A217:E217"/>
+    <mergeCell ref="A63:E63"/>
+    <mergeCell ref="A75:E75"/>
+    <mergeCell ref="A83:E83"/>
+    <mergeCell ref="A89:E89"/>
+    <mergeCell ref="A206:E206"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9757,84 +9762,84 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="F2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>580</v>
+      </c>
+      <c r="B3" t="s">
+        <v>585</v>
+      </c>
+      <c r="C3" t="s">
+        <v>592</v>
+      </c>
+      <c r="D3" t="s">
+        <v>584</v>
+      </c>
+      <c r="E3" t="s">
         <v>581</v>
       </c>
-      <c r="B3" t="s">
-        <v>586</v>
-      </c>
-      <c r="C3" t="s">
-        <v>593</v>
-      </c>
-      <c r="D3" t="s">
-        <v>585</v>
-      </c>
-      <c r="E3" t="s">
-        <v>582</v>
-      </c>
       <c r="F3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="30" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B5" s="30"/>
       <c r="C5" s="30"/>
       <c r="D5" s="30" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E5" s="30"/>
       <c r="F5" s="30"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="52.5" customHeight="1">
       <c r="A9" s="24" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="24"/>

</xml_diff>